<commit_message>
average function complexities has been added to xlsxContracts data
</commit_message>
<xml_diff>
--- a/sheets/xlsxContracts.xlsx
+++ b/sheets/xlsxContracts.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L77"/>
+  <dimension ref="A1:Z77"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -439,6 +439,48 @@
       <c r="L1" t="str">
         <v>Number of inherited classes</v>
       </c>
+      <c r="M1" t="str">
+        <v>Number of modifiers</v>
+      </c>
+      <c r="N1" t="str">
+        <v>Number of mappings</v>
+      </c>
+      <c r="O1" t="str">
+        <v>Number of arrays</v>
+      </c>
+      <c r="P1" t="str">
+        <v>Number of enums</v>
+      </c>
+      <c r="Q1" t="str">
+        <v>Number of public functions</v>
+      </c>
+      <c r="R1" t="str">
+        <v>Number of private functions</v>
+      </c>
+      <c r="S1" t="str">
+        <v>Number of internal functions</v>
+      </c>
+      <c r="T1" t="str">
+        <v>Number of external functions</v>
+      </c>
+      <c r="U1" t="str">
+        <v>Number of default functions</v>
+      </c>
+      <c r="V1" t="str">
+        <v>Number of constant state variables</v>
+      </c>
+      <c r="W1" t="str">
+        <v>Cyclomatic Complexity</v>
+      </c>
+      <c r="X1" t="str">
+        <v>Number of fallback functions</v>
+      </c>
+      <c r="Y1" t="str">
+        <v>Number of receive functions</v>
+      </c>
+      <c r="Z1" t="str">
+        <v>Number of function calls</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -477,6 +519,48 @@
       <c r="L2">
         <v>2</v>
       </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>2</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>24</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>56</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -515,6 +599,48 @@
       <c r="L3">
         <v>2</v>
       </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>5</v>
+      </c>
+      <c r="T3">
+        <v>4</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>53</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>153</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -553,6 +679,48 @@
       <c r="L4">
         <v>2</v>
       </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>6</v>
+      </c>
+      <c r="U4">
+        <v>1</v>
+      </c>
+      <c r="V4">
+        <v>3</v>
+      </c>
+      <c r="W4">
+        <v>4</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>16</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -591,6 +759,48 @@
       <c r="L5">
         <v>2</v>
       </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
+      <c r="T5">
+        <v>1</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>8</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>35</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -629,6 +839,48 @@
       <c r="L6">
         <v>1</v>
       </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>6</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>21</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>61</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -667,6 +919,48 @@
       <c r="L7">
         <v>1</v>
       </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>4</v>
+      </c>
+      <c r="T7">
+        <v>11</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>4</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>31</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -705,6 +999,48 @@
       <c r="L8">
         <v>1</v>
       </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <v>26</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>19</v>
+      </c>
+      <c r="X8">
+        <v>0</v>
+      </c>
+      <c r="Y8">
+        <v>0</v>
+      </c>
+      <c r="Z8">
+        <v>85</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -743,6 +1079,48 @@
       <c r="L9">
         <v>2</v>
       </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>14</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>1</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>1</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -781,6 +1159,48 @@
       <c r="L10">
         <v>1</v>
       </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>13</v>
+      </c>
+      <c r="T10">
+        <v>4</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>23</v>
+      </c>
+      <c r="X10">
+        <v>0</v>
+      </c>
+      <c r="Y10">
+        <v>0</v>
+      </c>
+      <c r="Z10">
+        <v>40</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -819,6 +1239,48 @@
       <c r="L11">
         <v>1</v>
       </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>4</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>3</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>21</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -857,6 +1319,48 @@
       <c r="L12">
         <v>0</v>
       </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>2</v>
+      </c>
+      <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>1</v>
+      </c>
+      <c r="X12">
+        <v>0</v>
+      </c>
+      <c r="Y12">
+        <v>0</v>
+      </c>
+      <c r="Z12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -895,6 +1399,48 @@
       <c r="L13">
         <v>0</v>
       </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>4</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <v>1</v>
+      </c>
+      <c r="X13">
+        <v>0</v>
+      </c>
+      <c r="Y13">
+        <v>0</v>
+      </c>
+      <c r="Z13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
@@ -933,6 +1479,48 @@
       <c r="L14">
         <v>0</v>
       </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>1</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <v>1</v>
+      </c>
+      <c r="X14">
+        <v>0</v>
+      </c>
+      <c r="Y14">
+        <v>0</v>
+      </c>
+      <c r="Z14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -971,6 +1559,48 @@
       <c r="L15">
         <v>0</v>
       </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>11</v>
+      </c>
+      <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>1</v>
+      </c>
+      <c r="X15">
+        <v>0</v>
+      </c>
+      <c r="Y15">
+        <v>0</v>
+      </c>
+      <c r="Z15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
@@ -1009,6 +1639,48 @@
       <c r="L16">
         <v>0</v>
       </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>1</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>1</v>
+      </c>
+      <c r="X16">
+        <v>0</v>
+      </c>
+      <c r="Y16">
+        <v>0</v>
+      </c>
+      <c r="Z16">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -1047,6 +1719,48 @@
       <c r="L17">
         <v>0</v>
       </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>69</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <v>1</v>
+      </c>
+      <c r="X17">
+        <v>0</v>
+      </c>
+      <c r="Y17">
+        <v>0</v>
+      </c>
+      <c r="Z17">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
@@ -1085,6 +1799,48 @@
       <c r="L18">
         <v>0</v>
       </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <v>1</v>
+      </c>
+      <c r="U18">
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <v>1</v>
+      </c>
+      <c r="X18">
+        <v>0</v>
+      </c>
+      <c r="Y18">
+        <v>0</v>
+      </c>
+      <c r="Z18">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
@@ -1123,6 +1879,48 @@
       <c r="L19">
         <v>0</v>
       </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <v>5</v>
+      </c>
+      <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19">
+        <v>1</v>
+      </c>
+      <c r="X19">
+        <v>0</v>
+      </c>
+      <c r="Y19">
+        <v>0</v>
+      </c>
+      <c r="Z19">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
@@ -1161,6 +1959,48 @@
       <c r="L20">
         <v>2</v>
       </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <v>6</v>
+      </c>
+      <c r="U20">
+        <v>0</v>
+      </c>
+      <c r="V20">
+        <v>0</v>
+      </c>
+      <c r="W20">
+        <v>1</v>
+      </c>
+      <c r="X20">
+        <v>0</v>
+      </c>
+      <c r="Y20">
+        <v>0</v>
+      </c>
+      <c r="Z20">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
@@ -1199,6 +2039,48 @@
       <c r="L21">
         <v>0</v>
       </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>5</v>
+      </c>
+      <c r="U21">
+        <v>0</v>
+      </c>
+      <c r="V21">
+        <v>0</v>
+      </c>
+      <c r="W21">
+        <v>1</v>
+      </c>
+      <c r="X21">
+        <v>0</v>
+      </c>
+      <c r="Y21">
+        <v>0</v>
+      </c>
+      <c r="Z21">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
@@ -1237,6 +2119,48 @@
       <c r="L22">
         <v>1</v>
       </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <v>0</v>
+      </c>
+      <c r="T22">
+        <v>10</v>
+      </c>
+      <c r="U22">
+        <v>0</v>
+      </c>
+      <c r="V22">
+        <v>0</v>
+      </c>
+      <c r="W22">
+        <v>1</v>
+      </c>
+      <c r="X22">
+        <v>0</v>
+      </c>
+      <c r="Y22">
+        <v>0</v>
+      </c>
+      <c r="Z22">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
@@ -1275,6 +2199,48 @@
       <c r="L23">
         <v>0</v>
       </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+      <c r="T23">
+        <v>6</v>
+      </c>
+      <c r="U23">
+        <v>0</v>
+      </c>
+      <c r="V23">
+        <v>0</v>
+      </c>
+      <c r="W23">
+        <v>1</v>
+      </c>
+      <c r="X23">
+        <v>0</v>
+      </c>
+      <c r="Y23">
+        <v>0</v>
+      </c>
+      <c r="Z23">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
@@ -1313,6 +2279,48 @@
       <c r="L24">
         <v>0</v>
       </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24">
+        <v>0</v>
+      </c>
+      <c r="R24">
+        <v>0</v>
+      </c>
+      <c r="S24">
+        <v>0</v>
+      </c>
+      <c r="T24">
+        <v>24</v>
+      </c>
+      <c r="U24">
+        <v>0</v>
+      </c>
+      <c r="V24">
+        <v>0</v>
+      </c>
+      <c r="W24">
+        <v>1</v>
+      </c>
+      <c r="X24">
+        <v>0</v>
+      </c>
+      <c r="Y24">
+        <v>0</v>
+      </c>
+      <c r="Z24">
+        <v>0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
@@ -1351,6 +2359,48 @@
       <c r="L25">
         <v>0</v>
       </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <v>0</v>
+      </c>
+      <c r="R25">
+        <v>0</v>
+      </c>
+      <c r="S25">
+        <v>0</v>
+      </c>
+      <c r="T25">
+        <v>19</v>
+      </c>
+      <c r="U25">
+        <v>0</v>
+      </c>
+      <c r="V25">
+        <v>0</v>
+      </c>
+      <c r="W25">
+        <v>1</v>
+      </c>
+      <c r="X25">
+        <v>0</v>
+      </c>
+      <c r="Y25">
+        <v>0</v>
+      </c>
+      <c r="Z25">
+        <v>0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
@@ -1389,6 +2439,48 @@
       <c r="L26">
         <v>0</v>
       </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <v>0</v>
+      </c>
+      <c r="R26">
+        <v>0</v>
+      </c>
+      <c r="S26">
+        <v>0</v>
+      </c>
+      <c r="T26">
+        <v>1</v>
+      </c>
+      <c r="U26">
+        <v>0</v>
+      </c>
+      <c r="V26">
+        <v>0</v>
+      </c>
+      <c r="W26">
+        <v>1</v>
+      </c>
+      <c r="X26">
+        <v>0</v>
+      </c>
+      <c r="Y26">
+        <v>0</v>
+      </c>
+      <c r="Z26">
+        <v>0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
@@ -1427,6 +2519,48 @@
       <c r="L27">
         <v>0</v>
       </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>0</v>
+      </c>
+      <c r="R27">
+        <v>0</v>
+      </c>
+      <c r="S27">
+        <v>0</v>
+      </c>
+      <c r="T27">
+        <v>3</v>
+      </c>
+      <c r="U27">
+        <v>0</v>
+      </c>
+      <c r="V27">
+        <v>0</v>
+      </c>
+      <c r="W27">
+        <v>1</v>
+      </c>
+      <c r="X27">
+        <v>0</v>
+      </c>
+      <c r="Y27">
+        <v>0</v>
+      </c>
+      <c r="Z27">
+        <v>0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
@@ -1465,6 +2599,48 @@
       <c r="L28">
         <v>1</v>
       </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <v>0</v>
+      </c>
+      <c r="Q28">
+        <v>0</v>
+      </c>
+      <c r="R28">
+        <v>0</v>
+      </c>
+      <c r="S28">
+        <v>0</v>
+      </c>
+      <c r="T28">
+        <v>5</v>
+      </c>
+      <c r="U28">
+        <v>0</v>
+      </c>
+      <c r="V28">
+        <v>0</v>
+      </c>
+      <c r="W28">
+        <v>1</v>
+      </c>
+      <c r="X28">
+        <v>0</v>
+      </c>
+      <c r="Y28">
+        <v>0</v>
+      </c>
+      <c r="Z28">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
@@ -1503,6 +2679,48 @@
       <c r="L29">
         <v>0</v>
       </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="N29">
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <v>0</v>
+      </c>
+      <c r="P29">
+        <v>0</v>
+      </c>
+      <c r="Q29">
+        <v>0</v>
+      </c>
+      <c r="R29">
+        <v>0</v>
+      </c>
+      <c r="S29">
+        <v>0</v>
+      </c>
+      <c r="T29">
+        <v>2</v>
+      </c>
+      <c r="U29">
+        <v>0</v>
+      </c>
+      <c r="V29">
+        <v>0</v>
+      </c>
+      <c r="W29">
+        <v>1</v>
+      </c>
+      <c r="X29">
+        <v>0</v>
+      </c>
+      <c r="Y29">
+        <v>0</v>
+      </c>
+      <c r="Z29">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
@@ -1541,6 +2759,48 @@
       <c r="L30">
         <v>1</v>
       </c>
+      <c r="M30">
+        <v>0</v>
+      </c>
+      <c r="N30">
+        <v>0</v>
+      </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <v>0</v>
+      </c>
+      <c r="Q30">
+        <v>0</v>
+      </c>
+      <c r="R30">
+        <v>0</v>
+      </c>
+      <c r="S30">
+        <v>2</v>
+      </c>
+      <c r="T30">
+        <v>3</v>
+      </c>
+      <c r="U30">
+        <v>0</v>
+      </c>
+      <c r="V30">
+        <v>0</v>
+      </c>
+      <c r="W30">
+        <v>2</v>
+      </c>
+      <c r="X30">
+        <v>0</v>
+      </c>
+      <c r="Y30">
+        <v>0</v>
+      </c>
+      <c r="Z30">
+        <v>22</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
@@ -1579,6 +2839,48 @@
       <c r="L31">
         <v>1</v>
       </c>
+      <c r="M31">
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <v>0</v>
+      </c>
+      <c r="R31">
+        <v>0</v>
+      </c>
+      <c r="S31">
+        <v>0</v>
+      </c>
+      <c r="T31">
+        <v>2</v>
+      </c>
+      <c r="U31">
+        <v>1</v>
+      </c>
+      <c r="V31">
+        <v>0</v>
+      </c>
+      <c r="W31">
+        <v>3</v>
+      </c>
+      <c r="X31">
+        <v>0</v>
+      </c>
+      <c r="Y31">
+        <v>0</v>
+      </c>
+      <c r="Z31">
+        <v>14</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
@@ -1617,6 +2919,48 @@
       <c r="L32">
         <v>1</v>
       </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <v>0</v>
+      </c>
+      <c r="O32">
+        <v>0</v>
+      </c>
+      <c r="P32">
+        <v>0</v>
+      </c>
+      <c r="Q32">
+        <v>0</v>
+      </c>
+      <c r="R32">
+        <v>0</v>
+      </c>
+      <c r="S32">
+        <v>0</v>
+      </c>
+      <c r="T32">
+        <v>0</v>
+      </c>
+      <c r="U32">
+        <v>1</v>
+      </c>
+      <c r="V32">
+        <v>4</v>
+      </c>
+      <c r="W32">
+        <v>1</v>
+      </c>
+      <c r="X32">
+        <v>0</v>
+      </c>
+      <c r="Y32">
+        <v>0</v>
+      </c>
+      <c r="Z32">
+        <v>6</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
@@ -1655,6 +2999,48 @@
       <c r="L33">
         <v>1</v>
       </c>
+      <c r="M33">
+        <v>0</v>
+      </c>
+      <c r="N33">
+        <v>0</v>
+      </c>
+      <c r="O33">
+        <v>0</v>
+      </c>
+      <c r="P33">
+        <v>0</v>
+      </c>
+      <c r="Q33">
+        <v>0</v>
+      </c>
+      <c r="R33">
+        <v>0</v>
+      </c>
+      <c r="S33">
+        <v>2</v>
+      </c>
+      <c r="T33">
+        <v>10</v>
+      </c>
+      <c r="U33">
+        <v>0</v>
+      </c>
+      <c r="V33">
+        <v>0</v>
+      </c>
+      <c r="W33">
+        <v>1</v>
+      </c>
+      <c r="X33">
+        <v>0</v>
+      </c>
+      <c r="Y33">
+        <v>0</v>
+      </c>
+      <c r="Z33">
+        <v>19</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
@@ -1693,6 +3079,48 @@
       <c r="L34">
         <v>1</v>
       </c>
+      <c r="M34">
+        <v>0</v>
+      </c>
+      <c r="N34">
+        <v>0</v>
+      </c>
+      <c r="O34">
+        <v>0</v>
+      </c>
+      <c r="P34">
+        <v>0</v>
+      </c>
+      <c r="Q34">
+        <v>3</v>
+      </c>
+      <c r="R34">
+        <v>0</v>
+      </c>
+      <c r="S34">
+        <v>5</v>
+      </c>
+      <c r="T34">
+        <v>4</v>
+      </c>
+      <c r="U34">
+        <v>0</v>
+      </c>
+      <c r="V34">
+        <v>0</v>
+      </c>
+      <c r="W34">
+        <v>16</v>
+      </c>
+      <c r="X34">
+        <v>0</v>
+      </c>
+      <c r="Y34">
+        <v>0</v>
+      </c>
+      <c r="Z34">
+        <v>71</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
@@ -1731,6 +3159,48 @@
       <c r="L35">
         <v>1</v>
       </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <v>0</v>
+      </c>
+      <c r="O35">
+        <v>0</v>
+      </c>
+      <c r="P35">
+        <v>0</v>
+      </c>
+      <c r="Q35">
+        <v>7</v>
+      </c>
+      <c r="R35">
+        <v>0</v>
+      </c>
+      <c r="S35">
+        <v>7</v>
+      </c>
+      <c r="T35">
+        <v>5</v>
+      </c>
+      <c r="U35">
+        <v>0</v>
+      </c>
+      <c r="V35">
+        <v>0</v>
+      </c>
+      <c r="W35">
+        <v>15</v>
+      </c>
+      <c r="X35">
+        <v>0</v>
+      </c>
+      <c r="Y35">
+        <v>0</v>
+      </c>
+      <c r="Z35">
+        <v>75</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
@@ -1769,6 +3239,48 @@
       <c r="L36">
         <v>0</v>
       </c>
+      <c r="M36">
+        <v>0</v>
+      </c>
+      <c r="N36">
+        <v>0</v>
+      </c>
+      <c r="O36">
+        <v>0</v>
+      </c>
+      <c r="P36">
+        <v>0</v>
+      </c>
+      <c r="Q36">
+        <v>0</v>
+      </c>
+      <c r="R36">
+        <v>0</v>
+      </c>
+      <c r="S36">
+        <v>0</v>
+      </c>
+      <c r="T36">
+        <v>41</v>
+      </c>
+      <c r="U36">
+        <v>0</v>
+      </c>
+      <c r="V36">
+        <v>0</v>
+      </c>
+      <c r="W36">
+        <v>1</v>
+      </c>
+      <c r="X36">
+        <v>0</v>
+      </c>
+      <c r="Y36">
+        <v>0</v>
+      </c>
+      <c r="Z36">
+        <v>0</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
@@ -1807,6 +3319,48 @@
       <c r="L37">
         <v>0</v>
       </c>
+      <c r="M37">
+        <v>0</v>
+      </c>
+      <c r="N37">
+        <v>0</v>
+      </c>
+      <c r="O37">
+        <v>0</v>
+      </c>
+      <c r="P37">
+        <v>0</v>
+      </c>
+      <c r="Q37">
+        <v>0</v>
+      </c>
+      <c r="R37">
+        <v>0</v>
+      </c>
+      <c r="S37">
+        <v>5</v>
+      </c>
+      <c r="T37">
+        <v>0</v>
+      </c>
+      <c r="U37">
+        <v>0</v>
+      </c>
+      <c r="V37">
+        <v>0</v>
+      </c>
+      <c r="W37">
+        <v>12</v>
+      </c>
+      <c r="X37">
+        <v>0</v>
+      </c>
+      <c r="Y37">
+        <v>0</v>
+      </c>
+      <c r="Z37">
+        <v>37</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
@@ -1845,6 +3399,48 @@
       <c r="L38">
         <v>0</v>
       </c>
+      <c r="M38">
+        <v>0</v>
+      </c>
+      <c r="N38">
+        <v>0</v>
+      </c>
+      <c r="O38">
+        <v>0</v>
+      </c>
+      <c r="P38">
+        <v>1</v>
+      </c>
+      <c r="Q38">
+        <v>0</v>
+      </c>
+      <c r="R38">
+        <v>0</v>
+      </c>
+      <c r="S38">
+        <v>0</v>
+      </c>
+      <c r="T38">
+        <v>0</v>
+      </c>
+      <c r="U38">
+        <v>0</v>
+      </c>
+      <c r="V38">
+        <v>0</v>
+      </c>
+      <c r="W38">
+        <v>1</v>
+      </c>
+      <c r="X38">
+        <v>0</v>
+      </c>
+      <c r="Y38">
+        <v>0</v>
+      </c>
+      <c r="Z38">
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
@@ -1883,6 +3479,48 @@
       <c r="L39">
         <v>0</v>
       </c>
+      <c r="M39">
+        <v>0</v>
+      </c>
+      <c r="N39">
+        <v>0</v>
+      </c>
+      <c r="O39">
+        <v>0</v>
+      </c>
+      <c r="P39">
+        <v>1</v>
+      </c>
+      <c r="Q39">
+        <v>0</v>
+      </c>
+      <c r="R39">
+        <v>0</v>
+      </c>
+      <c r="S39">
+        <v>0</v>
+      </c>
+      <c r="T39">
+        <v>0</v>
+      </c>
+      <c r="U39">
+        <v>0</v>
+      </c>
+      <c r="V39">
+        <v>0</v>
+      </c>
+      <c r="W39">
+        <v>1</v>
+      </c>
+      <c r="X39">
+        <v>0</v>
+      </c>
+      <c r="Y39">
+        <v>0</v>
+      </c>
+      <c r="Z39">
+        <v>0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
@@ -1921,6 +3559,48 @@
       <c r="L40">
         <v>0</v>
       </c>
+      <c r="M40">
+        <v>0</v>
+      </c>
+      <c r="N40">
+        <v>0</v>
+      </c>
+      <c r="O40">
+        <v>0</v>
+      </c>
+      <c r="P40">
+        <v>1</v>
+      </c>
+      <c r="Q40">
+        <v>0</v>
+      </c>
+      <c r="R40">
+        <v>0</v>
+      </c>
+      <c r="S40">
+        <v>0</v>
+      </c>
+      <c r="T40">
+        <v>0</v>
+      </c>
+      <c r="U40">
+        <v>0</v>
+      </c>
+      <c r="V40">
+        <v>0</v>
+      </c>
+      <c r="W40">
+        <v>1</v>
+      </c>
+      <c r="X40">
+        <v>0</v>
+      </c>
+      <c r="Y40">
+        <v>0</v>
+      </c>
+      <c r="Z40">
+        <v>0</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
@@ -1959,6 +3639,48 @@
       <c r="L41">
         <v>0</v>
       </c>
+      <c r="M41">
+        <v>0</v>
+      </c>
+      <c r="N41">
+        <v>0</v>
+      </c>
+      <c r="O41">
+        <v>0</v>
+      </c>
+      <c r="P41">
+        <v>0</v>
+      </c>
+      <c r="Q41">
+        <v>0</v>
+      </c>
+      <c r="R41">
+        <v>0</v>
+      </c>
+      <c r="S41">
+        <v>22</v>
+      </c>
+      <c r="T41">
+        <v>0</v>
+      </c>
+      <c r="U41">
+        <v>0</v>
+      </c>
+      <c r="V41">
+        <v>0</v>
+      </c>
+      <c r="W41">
+        <v>6</v>
+      </c>
+      <c r="X41">
+        <v>0</v>
+      </c>
+      <c r="Y41">
+        <v>0</v>
+      </c>
+      <c r="Z41">
+        <v>9</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
@@ -1997,6 +3719,48 @@
       <c r="L42">
         <v>0</v>
       </c>
+      <c r="M42">
+        <v>0</v>
+      </c>
+      <c r="N42">
+        <v>0</v>
+      </c>
+      <c r="O42">
+        <v>0</v>
+      </c>
+      <c r="P42">
+        <v>0</v>
+      </c>
+      <c r="Q42">
+        <v>0</v>
+      </c>
+      <c r="R42">
+        <v>0</v>
+      </c>
+      <c r="S42">
+        <v>1</v>
+      </c>
+      <c r="T42">
+        <v>0</v>
+      </c>
+      <c r="U42">
+        <v>0</v>
+      </c>
+      <c r="V42">
+        <v>0</v>
+      </c>
+      <c r="W42">
+        <v>1</v>
+      </c>
+      <c r="X42">
+        <v>0</v>
+      </c>
+      <c r="Y42">
+        <v>0</v>
+      </c>
+      <c r="Z42">
+        <v>0</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
@@ -2035,6 +3799,48 @@
       <c r="L43">
         <v>1</v>
       </c>
+      <c r="M43">
+        <v>0</v>
+      </c>
+      <c r="N43">
+        <v>1</v>
+      </c>
+      <c r="O43">
+        <v>0</v>
+      </c>
+      <c r="P43">
+        <v>0</v>
+      </c>
+      <c r="Q43">
+        <v>0</v>
+      </c>
+      <c r="R43">
+        <v>0</v>
+      </c>
+      <c r="S43">
+        <v>0</v>
+      </c>
+      <c r="T43">
+        <v>3</v>
+      </c>
+      <c r="U43">
+        <v>1</v>
+      </c>
+      <c r="V43">
+        <v>1</v>
+      </c>
+      <c r="W43">
+        <v>4</v>
+      </c>
+      <c r="X43">
+        <v>0</v>
+      </c>
+      <c r="Y43">
+        <v>0</v>
+      </c>
+      <c r="Z43">
+        <v>13</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
@@ -2073,6 +3879,48 @@
       <c r="L44">
         <v>1</v>
       </c>
+      <c r="M44">
+        <v>0</v>
+      </c>
+      <c r="N44">
+        <v>0</v>
+      </c>
+      <c r="O44">
+        <v>0</v>
+      </c>
+      <c r="P44">
+        <v>0</v>
+      </c>
+      <c r="Q44">
+        <v>0</v>
+      </c>
+      <c r="R44">
+        <v>0</v>
+      </c>
+      <c r="S44">
+        <v>0</v>
+      </c>
+      <c r="T44">
+        <v>1</v>
+      </c>
+      <c r="U44">
+        <v>1</v>
+      </c>
+      <c r="V44">
+        <v>0</v>
+      </c>
+      <c r="W44">
+        <v>1</v>
+      </c>
+      <c r="X44">
+        <v>0</v>
+      </c>
+      <c r="Y44">
+        <v>0</v>
+      </c>
+      <c r="Z44">
+        <v>1</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
@@ -2111,6 +3959,48 @@
       <c r="L45">
         <v>2</v>
       </c>
+      <c r="M45">
+        <v>0</v>
+      </c>
+      <c r="N45">
+        <v>0</v>
+      </c>
+      <c r="O45">
+        <v>0</v>
+      </c>
+      <c r="P45">
+        <v>0</v>
+      </c>
+      <c r="Q45">
+        <v>0</v>
+      </c>
+      <c r="R45">
+        <v>0</v>
+      </c>
+      <c r="S45">
+        <v>0</v>
+      </c>
+      <c r="T45">
+        <v>6</v>
+      </c>
+      <c r="U45">
+        <v>1</v>
+      </c>
+      <c r="V45">
+        <v>3</v>
+      </c>
+      <c r="W45">
+        <v>4</v>
+      </c>
+      <c r="X45">
+        <v>0</v>
+      </c>
+      <c r="Y45">
+        <v>0</v>
+      </c>
+      <c r="Z45">
+        <v>19</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
@@ -2149,6 +4039,48 @@
       <c r="L46">
         <v>2</v>
       </c>
+      <c r="M46">
+        <v>0</v>
+      </c>
+      <c r="N46">
+        <v>0</v>
+      </c>
+      <c r="O46">
+        <v>0</v>
+      </c>
+      <c r="P46">
+        <v>0</v>
+      </c>
+      <c r="Q46">
+        <v>0</v>
+      </c>
+      <c r="R46">
+        <v>0</v>
+      </c>
+      <c r="S46">
+        <v>1</v>
+      </c>
+      <c r="T46">
+        <v>1</v>
+      </c>
+      <c r="U46">
+        <v>0</v>
+      </c>
+      <c r="V46">
+        <v>0</v>
+      </c>
+      <c r="W46">
+        <v>7</v>
+      </c>
+      <c r="X46">
+        <v>0</v>
+      </c>
+      <c r="Y46">
+        <v>0</v>
+      </c>
+      <c r="Z46">
+        <v>31</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
@@ -2187,6 +4119,48 @@
       <c r="L47">
         <v>1</v>
       </c>
+      <c r="M47">
+        <v>0</v>
+      </c>
+      <c r="N47">
+        <v>0</v>
+      </c>
+      <c r="O47">
+        <v>0</v>
+      </c>
+      <c r="P47">
+        <v>0</v>
+      </c>
+      <c r="Q47">
+        <v>0</v>
+      </c>
+      <c r="R47">
+        <v>0</v>
+      </c>
+      <c r="S47">
+        <v>6</v>
+      </c>
+      <c r="T47">
+        <v>0</v>
+      </c>
+      <c r="U47">
+        <v>0</v>
+      </c>
+      <c r="V47">
+        <v>0</v>
+      </c>
+      <c r="W47">
+        <v>39</v>
+      </c>
+      <c r="X47">
+        <v>0</v>
+      </c>
+      <c r="Y47">
+        <v>0</v>
+      </c>
+      <c r="Z47">
+        <v>64</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
@@ -2225,6 +4199,48 @@
       <c r="L48">
         <v>1</v>
       </c>
+      <c r="M48">
+        <v>0</v>
+      </c>
+      <c r="N48">
+        <v>0</v>
+      </c>
+      <c r="O48">
+        <v>0</v>
+      </c>
+      <c r="P48">
+        <v>0</v>
+      </c>
+      <c r="Q48">
+        <v>0</v>
+      </c>
+      <c r="R48">
+        <v>0</v>
+      </c>
+      <c r="S48">
+        <v>4</v>
+      </c>
+      <c r="T48">
+        <v>12</v>
+      </c>
+      <c r="U48">
+        <v>0</v>
+      </c>
+      <c r="V48">
+        <v>0</v>
+      </c>
+      <c r="W48">
+        <v>4</v>
+      </c>
+      <c r="X48">
+        <v>0</v>
+      </c>
+      <c r="Y48">
+        <v>1</v>
+      </c>
+      <c r="Z48">
+        <v>35</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
@@ -2263,6 +4279,48 @@
       <c r="L49">
         <v>1</v>
       </c>
+      <c r="M49">
+        <v>0</v>
+      </c>
+      <c r="N49">
+        <v>0</v>
+      </c>
+      <c r="O49">
+        <v>0</v>
+      </c>
+      <c r="P49">
+        <v>0</v>
+      </c>
+      <c r="Q49">
+        <v>0</v>
+      </c>
+      <c r="R49">
+        <v>0</v>
+      </c>
+      <c r="S49">
+        <v>1</v>
+      </c>
+      <c r="T49">
+        <v>24</v>
+      </c>
+      <c r="U49">
+        <v>0</v>
+      </c>
+      <c r="V49">
+        <v>0</v>
+      </c>
+      <c r="W49">
+        <v>15</v>
+      </c>
+      <c r="X49">
+        <v>0</v>
+      </c>
+      <c r="Y49">
+        <v>0</v>
+      </c>
+      <c r="Z49">
+        <v>71</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
@@ -2301,6 +4359,48 @@
       <c r="L50">
         <v>2</v>
       </c>
+      <c r="M50">
+        <v>0</v>
+      </c>
+      <c r="N50">
+        <v>17</v>
+      </c>
+      <c r="O50">
+        <v>1</v>
+      </c>
+      <c r="P50">
+        <v>0</v>
+      </c>
+      <c r="Q50">
+        <v>0</v>
+      </c>
+      <c r="R50">
+        <v>0</v>
+      </c>
+      <c r="S50">
+        <v>0</v>
+      </c>
+      <c r="T50">
+        <v>0</v>
+      </c>
+      <c r="U50">
+        <v>1</v>
+      </c>
+      <c r="V50">
+        <v>0</v>
+      </c>
+      <c r="W50">
+        <v>1</v>
+      </c>
+      <c r="X50">
+        <v>0</v>
+      </c>
+      <c r="Y50">
+        <v>0</v>
+      </c>
+      <c r="Z50">
+        <v>0</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
@@ -2339,6 +4439,48 @@
       <c r="L51">
         <v>1</v>
       </c>
+      <c r="M51">
+        <v>1</v>
+      </c>
+      <c r="N51">
+        <v>0</v>
+      </c>
+      <c r="O51">
+        <v>0</v>
+      </c>
+      <c r="P51">
+        <v>0</v>
+      </c>
+      <c r="Q51">
+        <v>0</v>
+      </c>
+      <c r="R51">
+        <v>0</v>
+      </c>
+      <c r="S51">
+        <v>6</v>
+      </c>
+      <c r="T51">
+        <v>5</v>
+      </c>
+      <c r="U51">
+        <v>0</v>
+      </c>
+      <c r="V51">
+        <v>0</v>
+      </c>
+      <c r="W51">
+        <v>16</v>
+      </c>
+      <c r="X51">
+        <v>0</v>
+      </c>
+      <c r="Y51">
+        <v>0</v>
+      </c>
+      <c r="Z51">
+        <v>39</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
@@ -2377,6 +4519,48 @@
       <c r="L52">
         <v>2</v>
       </c>
+      <c r="M52">
+        <v>0</v>
+      </c>
+      <c r="N52">
+        <v>0</v>
+      </c>
+      <c r="O52">
+        <v>0</v>
+      </c>
+      <c r="P52">
+        <v>0</v>
+      </c>
+      <c r="Q52">
+        <v>0</v>
+      </c>
+      <c r="R52">
+        <v>0</v>
+      </c>
+      <c r="S52">
+        <v>9</v>
+      </c>
+      <c r="T52">
+        <v>6</v>
+      </c>
+      <c r="U52">
+        <v>0</v>
+      </c>
+      <c r="V52">
+        <v>0</v>
+      </c>
+      <c r="W52">
+        <v>99</v>
+      </c>
+      <c r="X52">
+        <v>0</v>
+      </c>
+      <c r="Y52">
+        <v>0</v>
+      </c>
+      <c r="Z52">
+        <v>241</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
@@ -2415,6 +4599,48 @@
       <c r="L53">
         <v>2</v>
       </c>
+      <c r="M53">
+        <v>1</v>
+      </c>
+      <c r="N53">
+        <v>5</v>
+      </c>
+      <c r="O53">
+        <v>0</v>
+      </c>
+      <c r="P53">
+        <v>0</v>
+      </c>
+      <c r="Q53">
+        <v>0</v>
+      </c>
+      <c r="R53">
+        <v>0</v>
+      </c>
+      <c r="S53">
+        <v>5</v>
+      </c>
+      <c r="T53">
+        <v>6</v>
+      </c>
+      <c r="U53">
+        <v>1</v>
+      </c>
+      <c r="V53">
+        <v>0</v>
+      </c>
+      <c r="W53">
+        <v>13</v>
+      </c>
+      <c r="X53">
+        <v>0</v>
+      </c>
+      <c r="Y53">
+        <v>0</v>
+      </c>
+      <c r="Z53">
+        <v>34</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
@@ -2453,6 +4679,48 @@
       <c r="L54">
         <v>0</v>
       </c>
+      <c r="M54">
+        <v>0</v>
+      </c>
+      <c r="N54">
+        <v>0</v>
+      </c>
+      <c r="O54">
+        <v>0</v>
+      </c>
+      <c r="P54">
+        <v>0</v>
+      </c>
+      <c r="Q54">
+        <v>0</v>
+      </c>
+      <c r="R54">
+        <v>0</v>
+      </c>
+      <c r="S54">
+        <v>0</v>
+      </c>
+      <c r="T54">
+        <v>11</v>
+      </c>
+      <c r="U54">
+        <v>0</v>
+      </c>
+      <c r="V54">
+        <v>0</v>
+      </c>
+      <c r="W54">
+        <v>1</v>
+      </c>
+      <c r="X54">
+        <v>0</v>
+      </c>
+      <c r="Y54">
+        <v>0</v>
+      </c>
+      <c r="Z54">
+        <v>0</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
@@ -2491,6 +4759,48 @@
       <c r="L55">
         <v>0</v>
       </c>
+      <c r="M55">
+        <v>0</v>
+      </c>
+      <c r="N55">
+        <v>0</v>
+      </c>
+      <c r="O55">
+        <v>0</v>
+      </c>
+      <c r="P55">
+        <v>0</v>
+      </c>
+      <c r="Q55">
+        <v>0</v>
+      </c>
+      <c r="R55">
+        <v>0</v>
+      </c>
+      <c r="S55">
+        <v>0</v>
+      </c>
+      <c r="T55">
+        <v>1</v>
+      </c>
+      <c r="U55">
+        <v>0</v>
+      </c>
+      <c r="V55">
+        <v>0</v>
+      </c>
+      <c r="W55">
+        <v>1</v>
+      </c>
+      <c r="X55">
+        <v>0</v>
+      </c>
+      <c r="Y55">
+        <v>0</v>
+      </c>
+      <c r="Z55">
+        <v>0</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
@@ -2529,6 +4839,48 @@
       <c r="L56">
         <v>0</v>
       </c>
+      <c r="M56">
+        <v>0</v>
+      </c>
+      <c r="N56">
+        <v>0</v>
+      </c>
+      <c r="O56">
+        <v>0</v>
+      </c>
+      <c r="P56">
+        <v>0</v>
+      </c>
+      <c r="Q56">
+        <v>0</v>
+      </c>
+      <c r="R56">
+        <v>0</v>
+      </c>
+      <c r="S56">
+        <v>0</v>
+      </c>
+      <c r="T56">
+        <v>62</v>
+      </c>
+      <c r="U56">
+        <v>0</v>
+      </c>
+      <c r="V56">
+        <v>0</v>
+      </c>
+      <c r="W56">
+        <v>1</v>
+      </c>
+      <c r="X56">
+        <v>0</v>
+      </c>
+      <c r="Y56">
+        <v>0</v>
+      </c>
+      <c r="Z56">
+        <v>0</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
@@ -2567,6 +4919,48 @@
       <c r="L57">
         <v>0</v>
       </c>
+      <c r="M57">
+        <v>0</v>
+      </c>
+      <c r="N57">
+        <v>0</v>
+      </c>
+      <c r="O57">
+        <v>0</v>
+      </c>
+      <c r="P57">
+        <v>0</v>
+      </c>
+      <c r="Q57">
+        <v>0</v>
+      </c>
+      <c r="R57">
+        <v>0</v>
+      </c>
+      <c r="S57">
+        <v>0</v>
+      </c>
+      <c r="T57">
+        <v>1</v>
+      </c>
+      <c r="U57">
+        <v>0</v>
+      </c>
+      <c r="V57">
+        <v>0</v>
+      </c>
+      <c r="W57">
+        <v>1</v>
+      </c>
+      <c r="X57">
+        <v>0</v>
+      </c>
+      <c r="Y57">
+        <v>0</v>
+      </c>
+      <c r="Z57">
+        <v>0</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
@@ -2605,6 +4999,48 @@
       <c r="L58">
         <v>0</v>
       </c>
+      <c r="M58">
+        <v>0</v>
+      </c>
+      <c r="N58">
+        <v>0</v>
+      </c>
+      <c r="O58">
+        <v>0</v>
+      </c>
+      <c r="P58">
+        <v>0</v>
+      </c>
+      <c r="Q58">
+        <v>0</v>
+      </c>
+      <c r="R58">
+        <v>0</v>
+      </c>
+      <c r="S58">
+        <v>0</v>
+      </c>
+      <c r="T58">
+        <v>6</v>
+      </c>
+      <c r="U58">
+        <v>0</v>
+      </c>
+      <c r="V58">
+        <v>0</v>
+      </c>
+      <c r="W58">
+        <v>1</v>
+      </c>
+      <c r="X58">
+        <v>0</v>
+      </c>
+      <c r="Y58">
+        <v>0</v>
+      </c>
+      <c r="Z58">
+        <v>0</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
@@ -2643,6 +5079,48 @@
       <c r="L59">
         <v>0</v>
       </c>
+      <c r="M59">
+        <v>0</v>
+      </c>
+      <c r="N59">
+        <v>0</v>
+      </c>
+      <c r="O59">
+        <v>0</v>
+      </c>
+      <c r="P59">
+        <v>0</v>
+      </c>
+      <c r="Q59">
+        <v>0</v>
+      </c>
+      <c r="R59">
+        <v>0</v>
+      </c>
+      <c r="S59">
+        <v>0</v>
+      </c>
+      <c r="T59">
+        <v>9</v>
+      </c>
+      <c r="U59">
+        <v>0</v>
+      </c>
+      <c r="V59">
+        <v>0</v>
+      </c>
+      <c r="W59">
+        <v>1</v>
+      </c>
+      <c r="X59">
+        <v>0</v>
+      </c>
+      <c r="Y59">
+        <v>0</v>
+      </c>
+      <c r="Z59">
+        <v>0</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
@@ -2681,6 +5159,48 @@
       <c r="L60">
         <v>0</v>
       </c>
+      <c r="M60">
+        <v>0</v>
+      </c>
+      <c r="N60">
+        <v>0</v>
+      </c>
+      <c r="O60">
+        <v>0</v>
+      </c>
+      <c r="P60">
+        <v>0</v>
+      </c>
+      <c r="Q60">
+        <v>0</v>
+      </c>
+      <c r="R60">
+        <v>0</v>
+      </c>
+      <c r="S60">
+        <v>0</v>
+      </c>
+      <c r="T60">
+        <v>2</v>
+      </c>
+      <c r="U60">
+        <v>0</v>
+      </c>
+      <c r="V60">
+        <v>0</v>
+      </c>
+      <c r="W60">
+        <v>1</v>
+      </c>
+      <c r="X60">
+        <v>0</v>
+      </c>
+      <c r="Y60">
+        <v>0</v>
+      </c>
+      <c r="Z60">
+        <v>0</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
@@ -2719,6 +5239,48 @@
       <c r="L61">
         <v>0</v>
       </c>
+      <c r="M61">
+        <v>0</v>
+      </c>
+      <c r="N61">
+        <v>0</v>
+      </c>
+      <c r="O61">
+        <v>0</v>
+      </c>
+      <c r="P61">
+        <v>0</v>
+      </c>
+      <c r="Q61">
+        <v>0</v>
+      </c>
+      <c r="R61">
+        <v>0</v>
+      </c>
+      <c r="S61">
+        <v>0</v>
+      </c>
+      <c r="T61">
+        <v>19</v>
+      </c>
+      <c r="U61">
+        <v>0</v>
+      </c>
+      <c r="V61">
+        <v>0</v>
+      </c>
+      <c r="W61">
+        <v>1</v>
+      </c>
+      <c r="X61">
+        <v>0</v>
+      </c>
+      <c r="Y61">
+        <v>0</v>
+      </c>
+      <c r="Z61">
+        <v>0</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
@@ -2757,6 +5319,48 @@
       <c r="L62">
         <v>0</v>
       </c>
+      <c r="M62">
+        <v>0</v>
+      </c>
+      <c r="N62">
+        <v>0</v>
+      </c>
+      <c r="O62">
+        <v>0</v>
+      </c>
+      <c r="P62">
+        <v>0</v>
+      </c>
+      <c r="Q62">
+        <v>0</v>
+      </c>
+      <c r="R62">
+        <v>0</v>
+      </c>
+      <c r="S62">
+        <v>0</v>
+      </c>
+      <c r="T62">
+        <v>43</v>
+      </c>
+      <c r="U62">
+        <v>0</v>
+      </c>
+      <c r="V62">
+        <v>0</v>
+      </c>
+      <c r="W62">
+        <v>1</v>
+      </c>
+      <c r="X62">
+        <v>0</v>
+      </c>
+      <c r="Y62">
+        <v>0</v>
+      </c>
+      <c r="Z62">
+        <v>0</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
@@ -2795,6 +5399,48 @@
       <c r="L63">
         <v>0</v>
       </c>
+      <c r="M63">
+        <v>0</v>
+      </c>
+      <c r="N63">
+        <v>0</v>
+      </c>
+      <c r="O63">
+        <v>0</v>
+      </c>
+      <c r="P63">
+        <v>0</v>
+      </c>
+      <c r="Q63">
+        <v>0</v>
+      </c>
+      <c r="R63">
+        <v>0</v>
+      </c>
+      <c r="S63">
+        <v>0</v>
+      </c>
+      <c r="T63">
+        <v>2</v>
+      </c>
+      <c r="U63">
+        <v>0</v>
+      </c>
+      <c r="V63">
+        <v>0</v>
+      </c>
+      <c r="W63">
+        <v>1</v>
+      </c>
+      <c r="X63">
+        <v>0</v>
+      </c>
+      <c r="Y63">
+        <v>0</v>
+      </c>
+      <c r="Z63">
+        <v>0</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
@@ -2833,6 +5479,48 @@
       <c r="L64">
         <v>0</v>
       </c>
+      <c r="M64">
+        <v>0</v>
+      </c>
+      <c r="N64">
+        <v>0</v>
+      </c>
+      <c r="O64">
+        <v>0</v>
+      </c>
+      <c r="P64">
+        <v>0</v>
+      </c>
+      <c r="Q64">
+        <v>0</v>
+      </c>
+      <c r="R64">
+        <v>0</v>
+      </c>
+      <c r="S64">
+        <v>0</v>
+      </c>
+      <c r="T64">
+        <v>39</v>
+      </c>
+      <c r="U64">
+        <v>0</v>
+      </c>
+      <c r="V64">
+        <v>0</v>
+      </c>
+      <c r="W64">
+        <v>1</v>
+      </c>
+      <c r="X64">
+        <v>0</v>
+      </c>
+      <c r="Y64">
+        <v>0</v>
+      </c>
+      <c r="Z64">
+        <v>0</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
@@ -2871,6 +5559,48 @@
       <c r="L65">
         <v>1</v>
       </c>
+      <c r="M65">
+        <v>0</v>
+      </c>
+      <c r="N65">
+        <v>0</v>
+      </c>
+      <c r="O65">
+        <v>0</v>
+      </c>
+      <c r="P65">
+        <v>0</v>
+      </c>
+      <c r="Q65">
+        <v>0</v>
+      </c>
+      <c r="R65">
+        <v>0</v>
+      </c>
+      <c r="S65">
+        <v>0</v>
+      </c>
+      <c r="T65">
+        <v>2</v>
+      </c>
+      <c r="U65">
+        <v>0</v>
+      </c>
+      <c r="V65">
+        <v>0</v>
+      </c>
+      <c r="W65">
+        <v>1</v>
+      </c>
+      <c r="X65">
+        <v>0</v>
+      </c>
+      <c r="Y65">
+        <v>0</v>
+      </c>
+      <c r="Z65">
+        <v>0</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
@@ -2909,6 +5639,48 @@
       <c r="L66">
         <v>0</v>
       </c>
+      <c r="M66">
+        <v>0</v>
+      </c>
+      <c r="N66">
+        <v>0</v>
+      </c>
+      <c r="O66">
+        <v>0</v>
+      </c>
+      <c r="P66">
+        <v>0</v>
+      </c>
+      <c r="Q66">
+        <v>0</v>
+      </c>
+      <c r="R66">
+        <v>0</v>
+      </c>
+      <c r="S66">
+        <v>0</v>
+      </c>
+      <c r="T66">
+        <v>1</v>
+      </c>
+      <c r="U66">
+        <v>0</v>
+      </c>
+      <c r="V66">
+        <v>0</v>
+      </c>
+      <c r="W66">
+        <v>1</v>
+      </c>
+      <c r="X66">
+        <v>0</v>
+      </c>
+      <c r="Y66">
+        <v>0</v>
+      </c>
+      <c r="Z66">
+        <v>0</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
@@ -2947,6 +5719,48 @@
       <c r="L67">
         <v>1</v>
       </c>
+      <c r="M67">
+        <v>0</v>
+      </c>
+      <c r="N67">
+        <v>0</v>
+      </c>
+      <c r="O67">
+        <v>0</v>
+      </c>
+      <c r="P67">
+        <v>0</v>
+      </c>
+      <c r="Q67">
+        <v>2</v>
+      </c>
+      <c r="R67">
+        <v>0</v>
+      </c>
+      <c r="S67">
+        <v>1</v>
+      </c>
+      <c r="T67">
+        <v>2</v>
+      </c>
+      <c r="U67">
+        <v>0</v>
+      </c>
+      <c r="V67">
+        <v>0</v>
+      </c>
+      <c r="W67">
+        <v>6</v>
+      </c>
+      <c r="X67">
+        <v>0</v>
+      </c>
+      <c r="Y67">
+        <v>0</v>
+      </c>
+      <c r="Z67">
+        <v>36</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="str">
@@ -2985,6 +5799,48 @@
       <c r="L68">
         <v>1</v>
       </c>
+      <c r="M68">
+        <v>0</v>
+      </c>
+      <c r="N68">
+        <v>0</v>
+      </c>
+      <c r="O68">
+        <v>0</v>
+      </c>
+      <c r="P68">
+        <v>0</v>
+      </c>
+      <c r="Q68">
+        <v>0</v>
+      </c>
+      <c r="R68">
+        <v>0</v>
+      </c>
+      <c r="S68">
+        <v>0</v>
+      </c>
+      <c r="T68">
+        <v>2</v>
+      </c>
+      <c r="U68">
+        <v>1</v>
+      </c>
+      <c r="V68">
+        <v>0</v>
+      </c>
+      <c r="W68">
+        <v>5</v>
+      </c>
+      <c r="X68">
+        <v>0</v>
+      </c>
+      <c r="Y68">
+        <v>0</v>
+      </c>
+      <c r="Z68">
+        <v>16</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
@@ -3023,6 +5879,48 @@
       <c r="L69">
         <v>2</v>
       </c>
+      <c r="M69">
+        <v>0</v>
+      </c>
+      <c r="N69">
+        <v>0</v>
+      </c>
+      <c r="O69">
+        <v>0</v>
+      </c>
+      <c r="P69">
+        <v>0</v>
+      </c>
+      <c r="Q69">
+        <v>0</v>
+      </c>
+      <c r="R69">
+        <v>0</v>
+      </c>
+      <c r="S69">
+        <v>0</v>
+      </c>
+      <c r="T69">
+        <v>0</v>
+      </c>
+      <c r="U69">
+        <v>1</v>
+      </c>
+      <c r="V69">
+        <v>3</v>
+      </c>
+      <c r="W69">
+        <v>1</v>
+      </c>
+      <c r="X69">
+        <v>0</v>
+      </c>
+      <c r="Y69">
+        <v>0</v>
+      </c>
+      <c r="Z69">
+        <v>5</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
@@ -3061,6 +5959,48 @@
       <c r="L70">
         <v>1</v>
       </c>
+      <c r="M70">
+        <v>0</v>
+      </c>
+      <c r="N70">
+        <v>0</v>
+      </c>
+      <c r="O70">
+        <v>0</v>
+      </c>
+      <c r="P70">
+        <v>0</v>
+      </c>
+      <c r="Q70">
+        <v>2</v>
+      </c>
+      <c r="R70">
+        <v>0</v>
+      </c>
+      <c r="S70">
+        <v>0</v>
+      </c>
+      <c r="T70">
+        <v>8</v>
+      </c>
+      <c r="U70">
+        <v>0</v>
+      </c>
+      <c r="V70">
+        <v>0</v>
+      </c>
+      <c r="W70">
+        <v>1</v>
+      </c>
+      <c r="X70">
+        <v>0</v>
+      </c>
+      <c r="Y70">
+        <v>0</v>
+      </c>
+      <c r="Z70">
+        <v>21</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
@@ -3099,6 +6039,48 @@
       <c r="L71">
         <v>1</v>
       </c>
+      <c r="M71">
+        <v>0</v>
+      </c>
+      <c r="N71">
+        <v>0</v>
+      </c>
+      <c r="O71">
+        <v>0</v>
+      </c>
+      <c r="P71">
+        <v>0</v>
+      </c>
+      <c r="Q71">
+        <v>3</v>
+      </c>
+      <c r="R71">
+        <v>0</v>
+      </c>
+      <c r="S71">
+        <v>5</v>
+      </c>
+      <c r="T71">
+        <v>4</v>
+      </c>
+      <c r="U71">
+        <v>0</v>
+      </c>
+      <c r="V71">
+        <v>0</v>
+      </c>
+      <c r="W71">
+        <v>16</v>
+      </c>
+      <c r="X71">
+        <v>0</v>
+      </c>
+      <c r="Y71">
+        <v>0</v>
+      </c>
+      <c r="Z71">
+        <v>89</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="str">
@@ -3137,6 +6119,48 @@
       <c r="L72">
         <v>1</v>
       </c>
+      <c r="M72">
+        <v>0</v>
+      </c>
+      <c r="N72">
+        <v>0</v>
+      </c>
+      <c r="O72">
+        <v>0</v>
+      </c>
+      <c r="P72">
+        <v>0</v>
+      </c>
+      <c r="Q72">
+        <v>4</v>
+      </c>
+      <c r="R72">
+        <v>0</v>
+      </c>
+      <c r="S72">
+        <v>0</v>
+      </c>
+      <c r="T72">
+        <v>3</v>
+      </c>
+      <c r="U72">
+        <v>0</v>
+      </c>
+      <c r="V72">
+        <v>0</v>
+      </c>
+      <c r="W72">
+        <v>11</v>
+      </c>
+      <c r="X72">
+        <v>0</v>
+      </c>
+      <c r="Y72">
+        <v>0</v>
+      </c>
+      <c r="Z72">
+        <v>28</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="str">
@@ -3175,6 +6199,48 @@
       <c r="L73">
         <v>1</v>
       </c>
+      <c r="M73">
+        <v>0</v>
+      </c>
+      <c r="N73">
+        <v>0</v>
+      </c>
+      <c r="O73">
+        <v>0</v>
+      </c>
+      <c r="P73">
+        <v>0</v>
+      </c>
+      <c r="Q73">
+        <v>7</v>
+      </c>
+      <c r="R73">
+        <v>0</v>
+      </c>
+      <c r="S73">
+        <v>3</v>
+      </c>
+      <c r="T73">
+        <v>5</v>
+      </c>
+      <c r="U73">
+        <v>0</v>
+      </c>
+      <c r="V73">
+        <v>0</v>
+      </c>
+      <c r="W73">
+        <v>21</v>
+      </c>
+      <c r="X73">
+        <v>0</v>
+      </c>
+      <c r="Y73">
+        <v>0</v>
+      </c>
+      <c r="Z73">
+        <v>78</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="str">
@@ -3213,6 +6279,48 @@
       <c r="L74">
         <v>0</v>
       </c>
+      <c r="M74">
+        <v>0</v>
+      </c>
+      <c r="N74">
+        <v>0</v>
+      </c>
+      <c r="O74">
+        <v>0</v>
+      </c>
+      <c r="P74">
+        <v>0</v>
+      </c>
+      <c r="Q74">
+        <v>0</v>
+      </c>
+      <c r="R74">
+        <v>0</v>
+      </c>
+      <c r="S74">
+        <v>0</v>
+      </c>
+      <c r="T74">
+        <v>44</v>
+      </c>
+      <c r="U74">
+        <v>0</v>
+      </c>
+      <c r="V74">
+        <v>0</v>
+      </c>
+      <c r="W74">
+        <v>1</v>
+      </c>
+      <c r="X74">
+        <v>0</v>
+      </c>
+      <c r="Y74">
+        <v>0</v>
+      </c>
+      <c r="Z74">
+        <v>0</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
@@ -3251,6 +6359,48 @@
       <c r="L75">
         <v>0</v>
       </c>
+      <c r="M75">
+        <v>0</v>
+      </c>
+      <c r="N75">
+        <v>0</v>
+      </c>
+      <c r="O75">
+        <v>0</v>
+      </c>
+      <c r="P75">
+        <v>0</v>
+      </c>
+      <c r="Q75">
+        <v>0</v>
+      </c>
+      <c r="R75">
+        <v>0</v>
+      </c>
+      <c r="S75">
+        <v>7</v>
+      </c>
+      <c r="T75">
+        <v>0</v>
+      </c>
+      <c r="U75">
+        <v>0</v>
+      </c>
+      <c r="V75">
+        <v>0</v>
+      </c>
+      <c r="W75">
+        <v>3</v>
+      </c>
+      <c r="X75">
+        <v>0</v>
+      </c>
+      <c r="Y75">
+        <v>0</v>
+      </c>
+      <c r="Z75">
+        <v>4</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
@@ -3289,6 +6439,48 @@
       <c r="L76">
         <v>0</v>
       </c>
+      <c r="M76">
+        <v>0</v>
+      </c>
+      <c r="N76">
+        <v>0</v>
+      </c>
+      <c r="O76">
+        <v>0</v>
+      </c>
+      <c r="P76">
+        <v>0</v>
+      </c>
+      <c r="Q76">
+        <v>0</v>
+      </c>
+      <c r="R76">
+        <v>0</v>
+      </c>
+      <c r="S76">
+        <v>5</v>
+      </c>
+      <c r="T76">
+        <v>0</v>
+      </c>
+      <c r="U76">
+        <v>0</v>
+      </c>
+      <c r="V76">
+        <v>0</v>
+      </c>
+      <c r="W76">
+        <v>10</v>
+      </c>
+      <c r="X76">
+        <v>0</v>
+      </c>
+      <c r="Y76">
+        <v>0</v>
+      </c>
+      <c r="Z76">
+        <v>33</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="str">
@@ -3327,10 +6519,52 @@
       <c r="L77">
         <v>0</v>
       </c>
+      <c r="M77">
+        <v>0</v>
+      </c>
+      <c r="N77">
+        <v>0</v>
+      </c>
+      <c r="O77">
+        <v>0</v>
+      </c>
+      <c r="P77">
+        <v>1</v>
+      </c>
+      <c r="Q77">
+        <v>0</v>
+      </c>
+      <c r="R77">
+        <v>0</v>
+      </c>
+      <c r="S77">
+        <v>0</v>
+      </c>
+      <c r="T77">
+        <v>0</v>
+      </c>
+      <c r="U77">
+        <v>0</v>
+      </c>
+      <c r="V77">
+        <v>0</v>
+      </c>
+      <c r="W77">
+        <v>1</v>
+      </c>
+      <c r="X77">
+        <v>0</v>
+      </c>
+      <c r="Y77">
+        <v>0</v>
+      </c>
+      <c r="Z77">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L77"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:Z77"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>